<commit_message>
Updated test cases precondition column
</commit_message>
<xml_diff>
--- a/Documentation/Eblocks - Online Calculator Test Cases.xlsx
+++ b/Documentation/Eblocks - Online Calculator Test Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakur/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakur/eclipse-workspace2/OnlineCalculator_Eblocks/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E0677-5193-CD43-A387-44BA9AD9DCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00042550-132D-F24F-86E2-BBD12E8C030B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{4A1DF33B-2771-2843-9F3C-273EF64B1E3C}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>TC007</t>
   </si>
   <si>
-    <t>Any updated web browser has been installed on your system. E.g Google chrome, Mozilla Firefox e.t.c)</t>
-  </si>
-  <si>
     <t>The calculator should return a value of 11 as the correct answer</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>EBLOCKS ONLINE CALCULATOR TEST CASES</t>
+  </si>
+  <si>
+    <t>An updated Google Chrome browser has been installed </t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -280,6 +280,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -319,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -472,11 +479,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,6 +551,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -499,50 +599,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,14 +933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BAD742-DBC5-4A42-B6E5-08A258D380E6}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="38" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="17" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="56.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -883,104 +956,104 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:77" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:77" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:77" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:77" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:77" ht="189" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:77" s="16" customFormat="1" ht="189" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="H6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:77" s="19" customFormat="1" ht="189" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1050,32 +1123,32 @@
       <c r="BX6" s="3"/>
       <c r="BY6" s="3"/>
     </row>
-    <row r="7" spans="1:77" s="19" customFormat="1" ht="189" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:77" s="16" customFormat="1" ht="189" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>18</v>
+      <c r="J7" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1145,32 +1218,32 @@
       <c r="BX7" s="3"/>
       <c r="BY7" s="3"/>
     </row>
-    <row r="8" spans="1:77" s="19" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:77" s="16" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="17" t="s">
+      <c r="I8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>18</v>
+      <c r="J8" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1240,32 +1313,32 @@
       <c r="BX8" s="3"/>
       <c r="BY8" s="3"/>
     </row>
-    <row r="9" spans="1:77" s="19" customFormat="1" ht="216" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:77" s="16" customFormat="1" ht="216" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>18</v>
+      <c r="J9" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1335,32 +1408,32 @@
       <c r="BX9" s="3"/>
       <c r="BY9" s="3"/>
     </row>
-    <row r="10" spans="1:77" s="19" customFormat="1" ht="189" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:77" s="16" customFormat="1" ht="189" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="G10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="17" t="s">
+      <c r="I10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>18</v>
+      <c r="J10" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1430,32 +1503,32 @@
       <c r="BX10" s="3"/>
       <c r="BY10" s="3"/>
     </row>
-    <row r="11" spans="1:77" s="19" customFormat="1" ht="189" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:77" s="16" customFormat="1" ht="189" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="I11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>18</v>
+      <c r="J11" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>

</xml_diff>